<commit_message>
Codebase which works for calculating MAT,YoY, TOPN , by brand grouping
</commit_message>
<xml_diff>
--- a/data/sample_nielsen_extended.xlsx
+++ b/data/sample_nielsen_extended.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T8567\Python related stuff\myproject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8894230D-9D65-466D-8056-A394DB3CD0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56784F1A-F51D-409B-91C0-1B655AB9C084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="44">
   <si>
     <t>date</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Sum of value_sales</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Dec</t>
+  </si>
+  <si>
+    <t>Sum of unit_sales</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8622,10 +8622,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5122A552-38F6-4CAA-8823-580AEF6EE75A}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:AO8" firstHeaderRow="1" firstDataRow="4" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5122A552-38F6-4CAA-8823-580AEF6EE75A}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:H17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField showAll="0">
       <items count="86">
         <item x="0"/>
         <item x="1"/>
@@ -8717,7 +8717,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="4">
         <item x="1"/>
         <item x="0"/>
@@ -8739,7 +8739,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0">
+    <pivotField showAll="0">
       <items count="674">
         <item x="171"/>
         <item x="163"/>
@@ -9417,7 +9417,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="86">
@@ -9509,10 +9509,10 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="15">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
+        <item x="1"/>
         <item sd="0" x="2"/>
         <item sd="0" x="3"/>
         <item sd="0" x="4"/>
@@ -9543,22 +9543,9 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="3"/>
+    <field x="9"/>
   </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="3">
-    <field x="10"/>
-    <field x="9"/>
-    <field x="0"/>
-  </colFields>
-  <colItems count="40">
+  <rowItems count="13">
     <i>
       <x v="1"/>
     </i>
@@ -9573,121 +9560,63 @@
     </i>
     <i>
       <x v="5"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
     </i>
     <i>
       <x v="6"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="10"/>
+  </colFields>
+  <colItems count="7">
+    <i>
       <x v="1"/>
     </i>
-    <i r="1">
+    <i>
       <x v="2"/>
     </i>
-    <i r="1">
+    <i>
       <x v="3"/>
     </i>
-    <i r="1">
+    <i>
       <x v="4"/>
     </i>
-    <i r="1">
+    <i>
       <x v="5"/>
     </i>
-    <i r="1">
+    <i>
       <x v="6"/>
     </i>
-    <i r="1">
+    <i>
       <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="4" item="0" hier="-1"/>
+    <pageField fld="4" item="4" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of value_sales" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of unit_sales" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -9988,8 +9917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I673"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A658" workbookViewId="0">
+      <selection activeCell="D672" sqref="D672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10020,7 +9949,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -30191,21 +30120,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EAAB9DC-CB91-4368-9050-AF81ACFC3A85}">
-  <dimension ref="A1:AS8"/>
+  <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="40" width="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="41" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="42" max="57" width="12" bestFit="1" customWidth="1"/>
     <col min="58" max="59" width="11" bestFit="1" customWidth="1"/>
     <col min="60" max="66" width="12" bestFit="1" customWidth="1"/>
@@ -30224,415 +30157,437 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="R4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" t="s">
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="B5" s="6">
+        <v>98766.7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>105006.56</v>
+      </c>
+      <c r="D5" s="6">
+        <v>103911.62</v>
+      </c>
+      <c r="E5" s="6">
+        <v>106478.15</v>
+      </c>
+      <c r="F5" s="6">
+        <v>118786.21</v>
+      </c>
+      <c r="G5" s="6">
+        <v>111001.31</v>
+      </c>
+      <c r="H5" s="6">
+        <v>111904.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>43</v>
-      </c>
-      <c r="R5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" t="s">
-        <v>35</v>
-      </c>
-      <c r="V5" t="s">
-        <v>36</v>
-      </c>
-      <c r="W5" t="s">
-        <v>37</v>
-      </c>
-      <c r="X5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
+      <c r="B6" s="6">
+        <v>105691.03</v>
+      </c>
+      <c r="C6" s="6">
+        <v>103426.08</v>
+      </c>
+      <c r="D6" s="6">
+        <v>109425.46</v>
+      </c>
+      <c r="E6" s="6">
+        <v>116916.82</v>
+      </c>
+      <c r="F6" s="6">
+        <v>108924.9</v>
+      </c>
+      <c r="G6" s="6">
+        <v>123180.2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>113897.4</v>
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
-        <v>14923926.529999997</v>
+        <v>111156.81</v>
       </c>
       <c r="C7" s="6">
-        <v>15367563.470000001</v>
+        <v>103772.36</v>
       </c>
       <c r="D7" s="6">
-        <v>16088774.409999998</v>
+        <v>106986.35</v>
       </c>
       <c r="E7" s="6">
-        <v>16340397.459999999</v>
+        <v>112154.96</v>
       </c>
       <c r="F7" s="6">
-        <v>1406790.29</v>
+        <v>119870.57</v>
       </c>
       <c r="G7" s="6">
-        <v>1605492.18</v>
+        <v>104289.45</v>
       </c>
       <c r="H7" s="6">
-        <v>1571654.64</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1510555.22</v>
-      </c>
-      <c r="J7" s="6">
-        <v>1443198.97</v>
-      </c>
-      <c r="K7" s="6">
-        <v>1486162.84</v>
-      </c>
-      <c r="L7" s="6">
-        <v>1249797.3700000001</v>
-      </c>
-      <c r="M7" s="6">
-        <v>1215457.8600000001</v>
-      </c>
-      <c r="N7" s="6">
-        <v>1320343.24</v>
-      </c>
-      <c r="O7" s="6">
-        <v>1281625.7</v>
-      </c>
-      <c r="P7" s="6">
-        <v>1396278.78</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>1470659.78</v>
-      </c>
-      <c r="R7" s="6">
-        <v>1538265.09</v>
-      </c>
-      <c r="S7" s="6">
-        <v>1499263.51</v>
-      </c>
-      <c r="T7" s="6">
-        <v>1538983.47</v>
-      </c>
-      <c r="U7" s="6">
-        <v>1542274.68</v>
-      </c>
-      <c r="V7" s="6">
-        <v>1463580.59</v>
-      </c>
-      <c r="W7" s="6">
-        <v>1433359.09</v>
-      </c>
-      <c r="X7" s="6">
-        <v>1382108.56</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>1372213.28</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>1272243.73</v>
-      </c>
-      <c r="AA7" s="6">
-        <v>1342837.77</v>
-      </c>
-      <c r="AB7" s="6">
-        <v>1374739.57</v>
-      </c>
-      <c r="AC7" s="6">
-        <v>1479050.97</v>
-      </c>
-      <c r="AD7" s="6">
-        <v>1585120.09</v>
-      </c>
-      <c r="AE7" s="6">
-        <v>1694270.52</v>
-      </c>
-      <c r="AF7" s="6">
-        <v>1554989.66</v>
-      </c>
-      <c r="AG7" s="6">
-        <v>1396913.87</v>
-      </c>
-      <c r="AH7" s="6">
-        <v>1375964.96</v>
-      </c>
-      <c r="AI7" s="6">
-        <v>1464044.37</v>
-      </c>
-      <c r="AJ7" s="6">
-        <v>1420659.95</v>
-      </c>
-      <c r="AK7" s="6">
-        <v>1267022.17</v>
-      </c>
-      <c r="AL7" s="6">
-        <v>1476702.29</v>
-      </c>
-      <c r="AM7" s="6">
-        <v>1386817.15</v>
-      </c>
-      <c r="AN7" s="6">
-        <v>1487601.17</v>
-      </c>
-      <c r="AO7" s="6">
-        <v>1544168.9</v>
+        <v>123942.24</v>
       </c>
       <c r="AQ7">
         <f>SUM(N7:Y7)</f>
-        <v>17238955.77</v>
+        <v>0</v>
       </c>
       <c r="AR7">
         <f>SUM(Z7:AK7)</f>
-        <v>17227857.630000003</v>
-      </c>
-      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="e">
         <f>AR7/AQ7-1</f>
-        <v>-6.4378261352182609E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6">
-        <v>14923926.529999997</v>
+        <v>105844.39</v>
       </c>
       <c r="C8" s="6">
-        <v>15367563.470000001</v>
+        <v>110406.02</v>
       </c>
       <c r="D8" s="6">
-        <v>16088774.409999998</v>
+        <v>114153.52</v>
       </c>
       <c r="E8" s="6">
-        <v>16340397.459999999</v>
+        <v>108056.52</v>
       </c>
       <c r="F8" s="6">
-        <v>1406790.29</v>
+        <v>123717.28</v>
       </c>
       <c r="G8" s="6">
-        <v>1605492.18</v>
+        <v>121063.22</v>
       </c>
       <c r="H8" s="6">
-        <v>1571654.64</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1510555.22</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1443198.97</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1486162.84</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1249797.3700000001</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1215457.8600000001</v>
-      </c>
-      <c r="N8" s="6">
-        <v>1320343.24</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1281625.7</v>
-      </c>
-      <c r="P8" s="6">
-        <v>1396278.78</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>1470659.78</v>
-      </c>
-      <c r="R8" s="6">
-        <v>1538265.09</v>
-      </c>
-      <c r="S8" s="6">
-        <v>1499263.51</v>
-      </c>
-      <c r="T8" s="6">
-        <v>1538983.47</v>
-      </c>
-      <c r="U8" s="6">
-        <v>1542274.68</v>
-      </c>
-      <c r="V8" s="6">
-        <v>1463580.59</v>
-      </c>
-      <c r="W8" s="6">
-        <v>1433359.09</v>
-      </c>
-      <c r="X8" s="6">
-        <v>1382108.56</v>
-      </c>
-      <c r="Y8" s="6">
-        <v>1372213.28</v>
-      </c>
-      <c r="Z8" s="6">
-        <v>1272243.73</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>1342837.77</v>
-      </c>
-      <c r="AB8" s="6">
-        <v>1374739.57</v>
-      </c>
-      <c r="AC8" s="6">
-        <v>1479050.97</v>
-      </c>
-      <c r="AD8" s="6">
-        <v>1585120.09</v>
-      </c>
-      <c r="AE8" s="6">
-        <v>1694270.52</v>
-      </c>
-      <c r="AF8" s="6">
-        <v>1554989.66</v>
-      </c>
-      <c r="AG8" s="6">
-        <v>1396913.87</v>
-      </c>
-      <c r="AH8" s="6">
-        <v>1375964.96</v>
-      </c>
-      <c r="AI8" s="6">
-        <v>1464044.37</v>
-      </c>
-      <c r="AJ8" s="6">
-        <v>1420659.95</v>
-      </c>
-      <c r="AK8" s="6">
-        <v>1267022.17</v>
-      </c>
-      <c r="AL8" s="6">
-        <v>1476702.29</v>
-      </c>
-      <c r="AM8" s="6">
-        <v>1386817.15</v>
-      </c>
-      <c r="AN8" s="6">
-        <v>1487601.17</v>
-      </c>
-      <c r="AO8" s="6">
-        <v>1544168.9</v>
+        <v>116024.39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6">
+        <v>97992.36</v>
+      </c>
+      <c r="C9" s="6">
+        <v>99330.78</v>
+      </c>
+      <c r="D9" s="6">
+        <v>116037.56</v>
+      </c>
+      <c r="E9" s="6">
+        <v>111254.41</v>
+      </c>
+      <c r="F9" s="6">
+        <v>112931.7</v>
+      </c>
+      <c r="G9" s="6">
+        <v>110441.59</v>
+      </c>
+      <c r="H9" s="6">
+        <v>125022.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6">
+        <v>87080.56</v>
+      </c>
+      <c r="C10" s="6">
+        <v>92795.47</v>
+      </c>
+      <c r="D10" s="6">
+        <v>99074.47</v>
+      </c>
+      <c r="E10" s="6">
+        <v>104941.97</v>
+      </c>
+      <c r="F10" s="6">
+        <v>113602.29</v>
+      </c>
+      <c r="G10" s="6">
+        <v>101943.63</v>
+      </c>
+      <c r="H10" s="6">
+        <v>113214.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="6">
+        <v>91974.8</v>
+      </c>
+      <c r="C11" s="6">
+        <v>89487.41</v>
+      </c>
+      <c r="D11" s="6">
+        <v>93762.35</v>
+      </c>
+      <c r="E11" s="6">
+        <v>98909.59</v>
+      </c>
+      <c r="F11" s="6">
+        <v>99466.04</v>
+      </c>
+      <c r="G11" s="6">
+        <v>108102.58</v>
+      </c>
+      <c r="H11" s="6">
+        <v>107998.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="6">
+        <v>84575.09</v>
+      </c>
+      <c r="C12" s="6">
+        <v>94220.92</v>
+      </c>
+      <c r="D12" s="6">
+        <v>95933.2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>97346.8</v>
+      </c>
+      <c r="F12" s="6">
+        <v>97197.1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>101010.65</v>
+      </c>
+      <c r="H12" s="6">
+        <v>99302.720000000001</v>
+      </c>
+      <c r="J12">
+        <f>GETPIVOTDATA("unit_sales",$A$3,"Months (date)",8,"Years (date)",2025)/GETPIVOTDATA("unit_sales",$A$3,"Months (date)",7,"Years (date)",2025)-1</f>
+        <v>-8.0520239065597132E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="6">
+        <v>89596.36</v>
+      </c>
+      <c r="C13" s="6">
+        <v>90794.17</v>
+      </c>
+      <c r="D13" s="6">
+        <v>92359.19</v>
+      </c>
+      <c r="E13" s="6">
+        <v>91427.19</v>
+      </c>
+      <c r="F13" s="6">
+        <v>94297.16</v>
+      </c>
+      <c r="G13" s="6">
+        <v>89568.53</v>
+      </c>
+      <c r="H13" s="6">
+        <v>102685.12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="6">
+        <v>90313.14</v>
+      </c>
+      <c r="C14" s="6">
+        <v>99719.86</v>
+      </c>
+      <c r="D14" s="6">
+        <v>95455.75</v>
+      </c>
+      <c r="E14" s="6">
+        <v>101925.46</v>
+      </c>
+      <c r="F14" s="6">
+        <v>104356.54</v>
+      </c>
+      <c r="G14" s="6">
+        <v>111168.31</v>
+      </c>
+      <c r="H14" s="6">
+        <v>103712.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="6">
+        <v>89897.33</v>
+      </c>
+      <c r="C15" s="6">
+        <v>98072.63</v>
+      </c>
+      <c r="D15" s="6">
+        <v>96059.91</v>
+      </c>
+      <c r="E15" s="6">
+        <v>99042.67</v>
+      </c>
+      <c r="F15" s="6">
+        <v>107399.38</v>
+      </c>
+      <c r="G15" s="6">
+        <v>105953.91</v>
+      </c>
+      <c r="H15" s="6">
+        <v>98127.6</v>
+      </c>
+      <c r="J15">
+        <f>(SUM(H5:H12)+SUM(G13:G16))/(SUM(G5:G12)+SUM(F13:F16))-1</f>
+        <v>1.5597215634027162E-2</v>
+      </c>
+      <c r="L15">
+        <f>(SUM(H5:H12)+SUM(G13:G16))</f>
+        <v>1320693.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="6">
+        <v>94845.95</v>
+      </c>
+      <c r="C16" s="6">
+        <v>102333.99</v>
+      </c>
+      <c r="D16" s="6">
+        <v>105672.91</v>
+      </c>
+      <c r="E16" s="6">
+        <v>113197.3</v>
+      </c>
+      <c r="F16" s="6">
+        <v>113325.24</v>
+      </c>
+      <c r="G16" s="6">
+        <v>102695.02</v>
+      </c>
+      <c r="H16" s="6">
+        <v>115806.81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1147734.52</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1189366.2500000002</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1228832.2899999998</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1261651.8399999999</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1313874.4099999999</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1290418.3999999999</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1331640.3400000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f>((SUM(H5:H12)+SUM(G13:G16)))</f>
+        <v>1320693.74</v>
+      </c>
+      <c r="G20">
+        <f>F20/F21-1</f>
+        <v>1.5597215634027162E-2</v>
+      </c>
+      <c r="I20">
+        <f>SUM(H5:H12)</f>
+        <v>911307.97</v>
+      </c>
+      <c r="J20">
+        <f>I20/I21-1</f>
+        <v>3.4363471872772777E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f>SUM(G5:G12)+SUM(F13:F16)</f>
+        <v>1300410.95</v>
+      </c>
+      <c r="I21">
+        <f>SUM(G5:G12)</f>
+        <v>881032.63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>GETPIVOTDATA("unit_sales",$A$3,"Months (date)",8,"Years (date)",2025)/GETPIVOTDATA("unit_sales",$A$3,"Months (date)",7,"Years (date)",2025)-1</f>
+        <v>-8.0520239065597132E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rule based insight generation system - does not have ytd/mat yoy window, basic ytd/mat,line chart peaks and only top 2 brands
</commit_message>
<xml_diff>
--- a/data/sample_nielsen_extended.xlsx
+++ b/data/sample_nielsen_extended.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T8567\Python related stuff\myproject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D2BECB-5A64-4CFE-93DC-B7D7ED4C2A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349ABC65-5317-4D17-9EC6-C651F7ECF3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="46">
   <si>
     <t>date</t>
   </si>
@@ -173,16 +172,13 @@
     <t>Dec</t>
   </si>
   <si>
-    <t>Sum of value_sales</t>
-  </si>
-  <si>
-    <t>(Multiple Items)</t>
-  </si>
-  <si>
     <t>MAT</t>
   </si>
   <si>
     <t>YTD</t>
+  </si>
+  <si>
+    <t>Sum of unit_sales</t>
   </si>
 </sst>
 </file>
@@ -7868,7 +7864,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5122A552-38F6-4CAA-8823-580AEF6EE75A}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5122A552-38F6-4CAA-8823-580AEF6EE75A}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField showAll="0">
@@ -7966,11 +7962,11 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="10">
-        <item x="0"/>
-        <item x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
         <item h="1" x="3"/>
         <item h="1" x="4"/>
-        <item h="1" x="2"/>
+        <item x="2"/>
         <item h="1" x="6"/>
         <item h="1" x="7"/>
         <item h="1" x="5"/>
@@ -7978,8 +7974,8 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -8089,7 +8085,7 @@
     <pageField fld="4" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of value_sales" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of unit_sales" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -21952,7 +21948,7 @@
         <v>22.78</v>
       </c>
       <c r="I452" t="str">
-        <f t="shared" ref="I451:I514" si="7">TEXT(A452,"mmm-yyyy")</f>
+        <f t="shared" ref="I452:I514" si="7">TEXT(A452,"mmm-yyyy")</f>
         <v>Sep-2023</v>
       </c>
     </row>
@@ -28603,20 +28599,24 @@
   <dimension ref="A1:AS25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F20" sqref="F20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.28515625" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="41" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="42" max="57" width="12" bestFit="1" customWidth="1"/>
     <col min="58" max="59" width="11" bestFit="1" customWidth="1"/>
     <col min="60" max="66" width="12" bestFit="1" customWidth="1"/>
@@ -28635,19 +28635,15 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="L3">
-        <f>SUM(F8:F10)/SUM(E8:E10)-1</f>
-        <v>2.4115642208110355E-2</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.25">
@@ -28681,25 +28677,25 @@
         <v>31</v>
       </c>
       <c r="B5" s="6">
-        <v>2359049.41</v>
+        <v>98766.7</v>
       </c>
       <c r="C5" s="6">
-        <v>2397689.04</v>
+        <v>105006.56</v>
       </c>
       <c r="D5" s="6">
-        <v>2373417.02</v>
+        <v>103911.62</v>
       </c>
       <c r="E5" s="6">
-        <v>2615124.25</v>
+        <v>106478.15</v>
       </c>
       <c r="F5" s="6">
-        <v>2606606.5300000003</v>
+        <v>118786.21</v>
       </c>
       <c r="G5" s="6">
-        <v>2865437.89</v>
+        <v>111001.31</v>
       </c>
       <c r="H5" s="6">
-        <v>2912754.67</v>
+        <v>111904.6</v>
       </c>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
@@ -28707,33 +28703,25 @@
         <v>32</v>
       </c>
       <c r="B6" s="6">
-        <v>2355941.94</v>
+        <v>105691.03</v>
       </c>
       <c r="C6" s="6">
-        <v>2459005.7400000002</v>
+        <v>103426.08</v>
       </c>
       <c r="D6" s="6">
-        <v>2656617.16</v>
+        <v>109425.46</v>
       </c>
       <c r="E6" s="6">
-        <v>2808947.3600000003</v>
+        <v>116916.82</v>
       </c>
       <c r="F6" s="6">
-        <v>2976295.65</v>
+        <v>108924.9</v>
       </c>
       <c r="G6" s="6">
-        <v>2761470.02</v>
+        <v>123180.2</v>
       </c>
       <c r="H6" s="6">
-        <v>3120977.89</v>
-      </c>
-      <c r="K6">
-        <f>SUM(F8:F10)</f>
-        <v>7962506.8399999999</v>
-      </c>
-      <c r="L6">
-        <f>K6/K7-1</f>
-        <v>2.4115642208110355E-2</v>
+        <v>113897.4</v>
       </c>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
@@ -28741,29 +28729,33 @@
         <v>33</v>
       </c>
       <c r="B7" s="6">
-        <v>2517127.21</v>
+        <v>111156.81</v>
       </c>
       <c r="C7" s="6">
-        <v>2449482.38</v>
+        <v>103772.36</v>
       </c>
       <c r="D7" s="6">
-        <v>2450444.2999999998</v>
+        <v>106986.35</v>
       </c>
       <c r="E7" s="6">
-        <v>2675101.9900000002</v>
+        <v>112154.96</v>
       </c>
       <c r="F7" s="6">
-        <v>2765257.5199999996</v>
+        <v>119870.57</v>
       </c>
       <c r="G7" s="6">
-        <v>2853069.33</v>
+        <v>104289.45</v>
       </c>
       <c r="H7" s="6">
-        <v>2738789.38</v>
+        <v>123942.24</v>
+      </c>
+      <c r="J7">
+        <f>SUM(F8:F10)</f>
+        <v>350251.26999999996</v>
       </c>
       <c r="K7">
         <f>SUM(E8:E10)</f>
-        <v>7775007.54</v>
+        <v>324252.90000000002</v>
       </c>
       <c r="AQ7">
         <f>SUM(N7:Y7)</f>
@@ -28783,25 +28775,29 @@
         <v>34</v>
       </c>
       <c r="B8" s="6">
-        <v>2438154.13</v>
+        <v>105844.39</v>
       </c>
       <c r="C8" s="6">
-        <v>2671333.2800000003</v>
+        <v>110406.02</v>
       </c>
       <c r="D8" s="6">
-        <v>2589351.4699999997</v>
+        <v>114153.52</v>
       </c>
       <c r="E8" s="6">
-        <v>2819985.6900000004</v>
+        <v>108056.52</v>
       </c>
       <c r="F8" s="6">
-        <v>2728248.41</v>
+        <v>123717.28</v>
       </c>
       <c r="G8" s="6">
-        <v>2771415.71</v>
+        <v>121063.22</v>
       </c>
       <c r="H8" s="6">
-        <v>2670384.12</v>
+        <v>116024.39</v>
+      </c>
+      <c r="J8">
+        <f>J7/K7-1</f>
+        <v>8.0179298319305481E-2</v>
       </c>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
@@ -28809,29 +28805,25 @@
         <v>35</v>
       </c>
       <c r="B9" s="6">
-        <v>2384119.44</v>
+        <v>97992.36</v>
       </c>
       <c r="C9" s="6">
-        <v>2450171.1500000004</v>
+        <v>99330.78</v>
       </c>
       <c r="D9" s="6">
-        <v>2573399.2400000002</v>
+        <v>116037.56</v>
       </c>
       <c r="E9" s="6">
-        <v>2507258.5999999996</v>
+        <v>111254.41</v>
       </c>
       <c r="F9" s="6">
-        <v>2595140.75</v>
+        <v>112931.7</v>
       </c>
       <c r="G9" s="6">
-        <v>2836374.3600000003</v>
+        <v>110441.59</v>
       </c>
       <c r="H9" s="6">
-        <v>2671967.48</v>
-      </c>
-      <c r="L9">
-        <f>SUM(F5:F16)</f>
-        <v>31121070.539999999</v>
+        <v>125022.89</v>
       </c>
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.25">
@@ -28839,25 +28831,25 @@
         <v>36</v>
       </c>
       <c r="B10" s="6">
-        <v>2329371.7599999998</v>
+        <v>87080.56</v>
       </c>
       <c r="C10" s="6">
-        <v>2482806.0300000003</v>
+        <v>92795.47</v>
       </c>
       <c r="D10" s="6">
-        <v>2634878.1800000002</v>
+        <v>99074.47</v>
       </c>
       <c r="E10" s="6">
-        <v>2447763.25</v>
+        <v>104941.97</v>
       </c>
       <c r="F10" s="6">
-        <v>2639117.6800000002</v>
+        <v>113602.29</v>
       </c>
       <c r="G10" s="6">
-        <v>2629216.7199999997</v>
+        <v>101943.63</v>
       </c>
       <c r="H10" s="6">
-        <v>2791650.74</v>
+        <v>113214.92</v>
       </c>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
@@ -28865,29 +28857,25 @@
         <v>37</v>
       </c>
       <c r="B11" s="6">
-        <v>2188379.1100000003</v>
+        <v>91974.8</v>
       </c>
       <c r="C11" s="6">
-        <v>2316361.5099999998</v>
+        <v>89487.41</v>
       </c>
       <c r="D11" s="6">
-        <v>2354451.5099999998</v>
+        <v>93762.35</v>
       </c>
       <c r="E11" s="6">
-        <v>2560795.5</v>
+        <v>98909.59</v>
       </c>
       <c r="F11" s="6">
-        <v>2349293.0300000003</v>
+        <v>99466.04</v>
       </c>
       <c r="G11" s="6">
-        <v>2558629.92</v>
+        <v>108102.58</v>
       </c>
       <c r="H11" s="6">
-        <v>2714284.17</v>
-      </c>
-      <c r="I11">
-        <f>SUM(F6:F16)</f>
-        <v>28514464.009999998</v>
+        <v>107998.81</v>
       </c>
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.25">
@@ -28895,29 +28883,25 @@
         <v>38</v>
       </c>
       <c r="B12" s="6">
-        <v>1996674.44</v>
+        <v>84575.09</v>
       </c>
       <c r="C12" s="6">
-        <v>2191541.16</v>
+        <v>94220.92</v>
       </c>
       <c r="D12" s="6">
-        <v>2242280.7599999998</v>
+        <v>95933.2</v>
       </c>
       <c r="E12" s="6">
-        <v>2339122.65</v>
+        <v>97346.8</v>
       </c>
       <c r="F12" s="6">
-        <v>2312031.89</v>
+        <v>97197.1</v>
       </c>
       <c r="G12" s="6">
-        <v>2487237.2000000002</v>
+        <v>101010.65</v>
       </c>
       <c r="H12" s="6">
-        <v>2392118.8499999996</v>
-      </c>
-      <c r="J12" t="e">
-        <f>GETPIVOTDATA("unit_sales",$A$3,"Months (date)",8,"Years (date)",2025)/GETPIVOTDATA("unit_sales",$A$3,"Months (date)",7,"Years (date)",2025)-1</f>
-        <v>#REF!</v>
+        <v>99302.720000000001</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
@@ -28925,25 +28909,25 @@
         <v>39</v>
       </c>
       <c r="B13" s="6">
-        <v>2203404.92</v>
+        <v>89596.36</v>
       </c>
       <c r="C13" s="6">
-        <v>2174337</v>
+        <v>90794.17</v>
       </c>
       <c r="D13" s="6">
-        <v>2320954.7599999998</v>
+        <v>92359.19</v>
       </c>
       <c r="E13" s="6">
-        <v>2149110.83</v>
+        <v>91427.19</v>
       </c>
       <c r="F13" s="6">
-        <v>2417319.29</v>
+        <v>94297.16</v>
       </c>
       <c r="G13" s="6">
-        <v>2392225.11</v>
+        <v>89568.53</v>
       </c>
       <c r="H13" s="6">
-        <v>2672265.9699999997</v>
+        <v>102685.12</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -28951,25 +28935,25 @@
         <v>40</v>
       </c>
       <c r="B14" s="6">
-        <v>2166301.8199999998</v>
+        <v>90313.14</v>
       </c>
       <c r="C14" s="6">
-        <v>2176325.77</v>
+        <v>99719.86</v>
       </c>
       <c r="D14" s="6">
-        <v>2390588.0499999998</v>
+        <v>95455.75</v>
       </c>
       <c r="E14" s="6">
-        <v>2450763.06</v>
+        <v>101925.46</v>
       </c>
       <c r="F14" s="6">
-        <v>2470080.56</v>
+        <v>104356.54</v>
       </c>
       <c r="G14" s="6">
-        <v>2473408.4699999997</v>
+        <v>111168.31</v>
       </c>
       <c r="H14" s="6">
-        <v>2488662.5</v>
+        <v>103712.84</v>
       </c>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
@@ -28977,33 +28961,25 @@
         <v>41</v>
       </c>
       <c r="B15" s="6">
-        <v>2349034.69</v>
+        <v>89897.33</v>
       </c>
       <c r="C15" s="6">
-        <v>2262059.5</v>
+        <v>98072.63</v>
       </c>
       <c r="D15" s="6">
-        <v>2317327.81</v>
+        <v>96059.91</v>
       </c>
       <c r="E15" s="6">
-        <v>2604719.46</v>
+        <v>99042.67</v>
       </c>
       <c r="F15" s="6">
-        <v>2562006.2400000002</v>
+        <v>107399.38</v>
       </c>
       <c r="G15" s="6">
-        <v>2628631.31</v>
+        <v>105953.91</v>
       </c>
       <c r="H15" s="6">
-        <v>2639840.63</v>
-      </c>
-      <c r="J15">
-        <f>(SUM(H5:H12)+SUM(G13:G16))/(SUM(G5:G12)+SUM(F13:F16))-1</f>
-        <v>7.9027538661051722E-3</v>
-      </c>
-      <c r="L15">
-        <f>(SUM(H5:H12)+SUM(G13:G16))</f>
-        <v>32164122.360000007</v>
+        <v>98127.6</v>
       </c>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
@@ -29011,25 +28987,25 @@
         <v>42</v>
       </c>
       <c r="B16" s="6">
-        <v>2392533.5499999998</v>
+        <v>94845.95</v>
       </c>
       <c r="C16" s="6">
-        <v>2293082.38</v>
+        <v>102333.99</v>
       </c>
       <c r="D16" s="6">
-        <v>2438417.1100000003</v>
+        <v>105672.91</v>
       </c>
       <c r="E16" s="6">
-        <v>2527611.3200000003</v>
+        <v>113197.3</v>
       </c>
       <c r="F16" s="6">
-        <v>2699672.99</v>
+        <v>113325.24</v>
       </c>
       <c r="G16" s="6">
-        <v>2656930.17</v>
+        <v>102695.02</v>
       </c>
       <c r="H16" s="6">
-        <v>2732261.54</v>
+        <v>115806.81</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -29037,67 +29013,75 @@
         <v>21</v>
       </c>
       <c r="B17" s="6">
-        <v>27680092.420000002</v>
+        <v>1147734.52</v>
       </c>
       <c r="C17" s="6">
-        <v>28324194.940000001</v>
+        <v>1189366.2500000002</v>
       </c>
       <c r="D17" s="6">
-        <v>29342127.369999997</v>
+        <v>1228832.2899999998</v>
       </c>
       <c r="E17" s="6">
-        <v>30506303.959999997</v>
+        <v>1261651.8399999999</v>
       </c>
       <c r="F17" s="6">
-        <v>31121070.539999999</v>
+        <v>1313874.4099999999</v>
       </c>
       <c r="G17" s="6">
-        <v>31914046.209999993</v>
+        <v>1290418.3999999999</v>
       </c>
       <c r="H17" s="6">
-        <v>32545957.940000001</v>
+        <v>1331640.3400000001</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="e">
+        <f>GETPIVOTDATA("value_sales",$A$3,"Months (date)",2,"Years (date)",2022)/GETPIVOTDATA("value_sales",$A$3,"Months (date)",1,"Years (date)",2022)-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D20">
+        <f>SUM(F5:F16)</f>
+        <v>1313874.4099999999</v>
+      </c>
       <c r="F20">
-        <f>((SUM(H5:H12)+SUM(G13:G16)))</f>
-        <v>32164122.360000007</v>
+        <f>((SUM(H5:H13)+SUM(G14:G16)))</f>
+        <v>1333810.33</v>
       </c>
       <c r="G20">
         <f>F20/F21-1</f>
-        <v>7.9027538661051722E-3</v>
+        <v>2.9426974044069798E-2</v>
       </c>
       <c r="I20">
-        <f>SUM(H5:H12)</f>
-        <v>22012927.300000004</v>
+        <f>SUM(H5:H13)</f>
+        <v>1013993.09</v>
       </c>
       <c r="J20">
         <f>I20/I21-1</f>
-        <v>1.1490964500761702E-2</v>
+        <v>4.4706241645126266E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21">
-        <f>SUM(G5:G12)+SUM(F13:F16)</f>
-        <v>31911930.229999997</v>
+        <f>SUM(G5:G13)+SUM(F14:F16)</f>
+        <v>1295682.32</v>
       </c>
       <c r="I21">
-        <f>SUM(G5:G12)</f>
-        <v>21762851.149999995</v>
+        <f>SUM(G5:G13)</f>
+        <v>970601.16</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G25" t="e">
+      <c r="G25">
         <f>GETPIVOTDATA("unit_sales",$A$3,"Months (date)",8,"Years (date)",2025)/GETPIVOTDATA("unit_sales",$A$3,"Months (date)",7,"Years (date)",2025)-1</f>
-        <v>#REF!</v>
+        <v>-8.0520239065597132E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>